<commit_message>
Uploaded new version of Income-Data
</commit_message>
<xml_diff>
--- a/Data sets/Income-Data.xlsx
+++ b/Data sets/Income-Data.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="county-level" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="state-level" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="income" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="state-level" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="12">
   <si>
     <t>State</t>
   </si>
@@ -35,19 +36,19 @@
     <t>MD</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
     <t>Pop</t>
   </si>
   <si>
     <t>Education</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -103,6 +104,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -507,7 +512,7 @@
       <c r="C12" s="1">
         <v>98.0</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>25.0</v>
       </c>
       <c r="E12" s="1">
@@ -653,7 +658,143 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>69.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>69.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>78.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>78.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>67.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -662,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -701,7 +842,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>5231.0</v>
@@ -718,7 +859,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>29587.0</v>
@@ -735,7 +876,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>18142.0</v>

</xml_diff>

<commit_message>
Added Pop column to income-data
</commit_message>
<xml_diff>
--- a/Data sets/Income-Data.xlsx
+++ b/Data sets/Income-Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t>State</t>
   </si>
@@ -36,6 +36,9 @@
     <t>MD</t>
   </si>
   <si>
+    <t>Pop</t>
+  </si>
+  <si>
     <t>IN</t>
   </si>
   <si>
@@ -43,9 +46,6 @@
   </si>
   <si>
     <t>NY</t>
-  </si>
-  <si>
-    <t>Pop</t>
   </si>
   <si>
     <t>Education</t>
@@ -663,6 +663,9 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -674,6 +677,9 @@
       <c r="C2" s="1">
         <v>69.0</v>
       </c>
+      <c r="D2" s="2">
+        <v>70.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -685,10 +691,13 @@
       <c r="C3" s="1">
         <v>35.0</v>
       </c>
+      <c r="D3" s="1">
+        <v>33.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>32.0</v>
@@ -696,10 +705,13 @@
       <c r="C4" s="1">
         <v>69.0</v>
       </c>
+      <c r="D4" s="2">
+        <v>23.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>35.0</v>
@@ -707,10 +719,13 @@
       <c r="C5" s="1">
         <v>54.0</v>
       </c>
+      <c r="D5" s="1">
+        <v>54.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>29.0</v>
@@ -718,6 +733,9 @@
       <c r="C6" s="1">
         <v>78.0</v>
       </c>
+      <c r="D6" s="1">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -729,6 +747,9 @@
       <c r="C7" s="1">
         <v>54.0</v>
       </c>
+      <c r="D7" s="2">
+        <v>27.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -740,10 +761,13 @@
       <c r="C8" s="1">
         <v>67.0</v>
       </c>
+      <c r="D8" s="2">
+        <v>81.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>41.0</v>
@@ -751,10 +775,13 @@
       <c r="C9" s="1">
         <v>35.0</v>
       </c>
+      <c r="D9" s="2">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>29.0</v>
@@ -762,16 +789,22 @@
       <c r="C10" s="1">
         <v>78.0</v>
       </c>
+      <c r="D10" s="2">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>34.0</v>
       </c>
       <c r="C11" s="1">
         <v>67.0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7.0</v>
       </c>
     </row>
   </sheetData>
@@ -794,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -842,7 +875,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>5231.0</v>
@@ -859,7 +892,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>29587.0</v>
@@ -876,7 +909,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>18142.0</v>

</xml_diff>